<commit_message>
Update with Hall_2015_2018 and Saiz_2015
</commit_message>
<xml_diff>
--- a/ISRaD_data_files/Wang_1999.xlsx
+++ b/ISRaD_data_files/Wang_1999.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -3048,13 +3048,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3339,13 +3344,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3395,7 +3400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3442,7 +3447,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3480,7 +3485,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3543,12 +3548,12 @@
       <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3571,7 +3576,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3611,7 +3616,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3647,13 +3652,13 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3763,7 +3768,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3873,7 +3878,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3968,7 +3973,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3994,7 +3999,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -4020,7 +4025,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -4063,9 +4068,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4178,7 +4183,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4288,7 +4293,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4387,12 +4392,12 @@
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4688,7 +4693,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="2" spans="1:98">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4984,7 +4989,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="3" spans="1:98">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5223,7 +5228,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="4" spans="1:98">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -5261,7 +5266,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="5" spans="1:98">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -5299,7 +5304,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="6" spans="1:98">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -5337,7 +5342,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="7" spans="1:98">
+    <row r="7" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -5375,7 +5380,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="8" spans="1:98">
+    <row r="8" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -5413,7 +5418,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="9" spans="1:98">
+    <row r="9" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -5451,7 +5456,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="10" spans="1:98">
+    <row r="10" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -5489,7 +5494,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="11" spans="1:98">
+    <row r="11" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -5527,7 +5532,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="12" spans="1:98">
+    <row r="12" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -5565,7 +5570,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="13" spans="1:98">
+    <row r="13" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -5603,7 +5608,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="14" spans="1:98">
+    <row r="14" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -5641,7 +5646,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="15" spans="1:98">
+    <row r="15" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -5679,7 +5684,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="1:98">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -5717,7 +5722,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="17" spans="1:56">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -5755,7 +5760,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="18" spans="1:56">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -5793,7 +5798,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="19" spans="1:56">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -5831,7 +5836,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="20" spans="1:56">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -5869,7 +5874,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="21" spans="1:56">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -5907,7 +5912,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="22" spans="1:56">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -5966,9 +5971,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6054,7 +6059,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6137,7 +6142,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -6199,13 +6204,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView topLeftCell="R1" workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AK1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:73" ht="52">
+    <row r="1" spans="1:73" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6426,7 +6431,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="2" spans="1:73">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6644,7 +6649,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="3" spans="1:73">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -6828,9 +6833,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6922,7 +6927,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -7005,7 +7010,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -7069,9 +7074,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>721</v>
       </c>
@@ -7205,7 +7210,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -7339,7 +7344,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="G3" t="s">
         <v>767</v>
       </c>
@@ -7362,7 +7367,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>772</v>
       </c>
@@ -7496,7 +7501,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>805</v>
       </c>
@@ -7609,7 +7614,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>838</v>
       </c>
@@ -7710,7 +7715,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>864</v>
       </c>
@@ -7784,7 +7789,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>885</v>
       </c>
@@ -7852,7 +7857,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>902</v>
       </c>
@@ -7905,7 +7910,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>918</v>
       </c>
@@ -7937,7 +7942,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>928</v>
       </c>
@@ -7963,7 +7968,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="H12" t="s">
         <v>935</v>
       </c>
@@ -7980,7 +7985,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U13" t="s">
         <v>940</v>
       </c>
@@ -7994,7 +7999,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U14" t="s">
         <v>944</v>
       </c>
@@ -8005,7 +8010,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U15" t="s">
         <v>947</v>
       </c>
@@ -8016,7 +8021,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U16" t="s">
         <v>950</v>
       </c>
@@ -8027,7 +8032,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="17" spans="40:41">
+    <row r="17" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN17" t="s">
         <v>953</v>
       </c>
@@ -8035,7 +8040,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="18" spans="40:41">
+    <row r="18" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN18" t="s">
         <v>955</v>
       </c>
@@ -8043,7 +8048,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="19" spans="40:41">
+    <row r="19" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN19" t="s">
         <v>957</v>
       </c>
@@ -8051,7 +8056,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="20" spans="40:41">
+    <row r="20" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN20" t="s">
         <v>959</v>
       </c>
@@ -8059,7 +8064,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="21" spans="40:41">
+    <row r="21" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN21" t="s">
         <v>961</v>
       </c>

</xml_diff>